<commit_message>
saving before running spokenenn / sign only models
</commit_message>
<xml_diff>
--- a/paper/tables/Table1.xlsx
+++ b/paper/tables/Table1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">CDI version</t>
   </si>
@@ -23,25 +23,31 @@
     <t xml:space="preserve">Mean Comprehension (SD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean Production (SD)</t>
+    <t xml:space="preserve">Mean Spoken Word Production (SD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean Sign Production (SD)</t>
   </si>
   <si>
     <t xml:space="preserve">% Developmental Delays</t>
   </si>
   <si>
-    <t xml:space="preserve">WG (n = 74)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.9 (8.8) months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105 (100) words</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32 (53) words</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.9%</t>
+    <t xml:space="preserve">WG (n = 75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.1 (8.9) months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106 (99) words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 (59) words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (2) words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.7%</t>
   </si>
   <si>
     <t xml:space="preserve">WS (n = 24)</t>
@@ -53,7 +59,10 @@
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">149 (180) words</t>
+    <t xml:space="preserve">138 (185) words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (0) words</t>
   </si>
   <si>
     <t xml:space="preserve">4.2%</t>
@@ -404,39 +413,48 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>